<commit_message>
Final version of submission
</commit_message>
<xml_diff>
--- a/HEMF Working Paper/Figures_Data_Preparation_9-12.xlsx
+++ b/HEMF Working Paper/Figures_Data_Preparation_9-12.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shakh\PycharmProjects\EWL-DUE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shakh\PycharmProjects\EWL-DUE\HEMF Working Paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DAFE8C4-29AF-4BD3-941D-D5A62ACCC9A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBFD603-B22B-4930-A43E-0B90D3BD6FFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="468" yWindow="228" windowWidth="22572" windowHeight="12732" activeTab="5" xr2:uid="{67C1415B-AAE7-42F9-A2F9-7B3268675C94}"/>
+    <workbookView xWindow="0" yWindow="996" windowWidth="21600" windowHeight="11508" activeTab="5" xr2:uid="{67C1415B-AAE7-42F9-A2F9-7B3268675C94}"/>
   </bookViews>
   <sheets>
     <sheet name="Figure 3" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="70">
   <si>
     <t>Figure 3: Generation capacities and power generation of the efficient portfolio under different instruments</t>
   </si>
@@ -245,6 +245,15 @@
   </si>
   <si>
     <t>Mixed</t>
+  </si>
+  <si>
+    <t>PV</t>
+  </si>
+  <si>
+    <t>Li-Ion</t>
+  </si>
+  <si>
+    <t>Hard Coal</t>
   </si>
 </sst>
 </file>
@@ -961,17 +970,17 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -981,7 +990,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
@@ -1007,7 +1016,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1033,7 +1042,7 @@
         <v>90.117406304368316</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
@@ -1059,7 +1068,7 @@
         <v>159.35673568418738</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
@@ -1085,7 +1094,7 @@
         <v>90.077492798125888</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
@@ -1111,7 +1120,7 @@
         <v>178.08111225000002</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>12</v>
       </c>
@@ -1137,7 +1146,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>7</v>
       </c>
@@ -1163,7 +1172,7 @@
         <v>81.10978467991049</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
@@ -1189,7 +1198,7 @@
         <v>143.42834585121994</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
         <v>9</v>
       </c>
@@ -1215,7 +1224,7 @@
         <v>81.073860699961401</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
@@ -1241,7 +1250,7 @@
         <v>160.28114059754415</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" s="4" t="s">
         <v>1</v>
       </c>
@@ -1249,7 +1258,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
         <v>7</v>
       </c>
@@ -1257,7 +1266,7 @@
         <v>90.034676750000003</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>8</v>
       </c>
@@ -1265,7 +1274,7 @@
         <v>90.034676750000003</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
         <v>9</v>
       </c>
@@ -1273,7 +1282,7 @@
         <v>90.034676750000003</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
         <v>10</v>
       </c>
@@ -1281,7 +1290,7 @@
         <v>90.034676750000003</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
         <v>1</v>
       </c>
@@ -1289,7 +1298,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
         <v>7</v>
       </c>
@@ -1297,7 +1306,7 @@
         <v>540.76861482299978</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" s="5" t="s">
         <v>8</v>
       </c>
@@ -1305,7 +1314,7 @@
         <v>540.76861482299978</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" s="5" t="s">
         <v>9</v>
       </c>
@@ -1313,7 +1322,7 @@
         <v>540.76861482299978</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28" s="5" t="s">
         <v>10</v>
       </c>
@@ -1335,17 +1344,17 @@
       <selection activeCell="A12" sqref="A12:A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
@@ -1356,7 +1365,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>7</v>
       </c>
@@ -1367,7 +1376,7 @@
         <v>13.742490026119633</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>8</v>
       </c>
@@ -1378,7 +1387,7 @@
         <v>35.574885252941264</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>9</v>
       </c>
@@ -1389,7 +1398,7 @@
         <v>13.759838932438845</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>10</v>
       </c>
@@ -1400,7 +1409,7 @@
         <v>22.144778190016886</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>20</v>
       </c>
@@ -1411,7 +1420,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>7</v>
       </c>
@@ -1422,7 +1431,7 @@
         <v>240.59692733201851</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>8</v>
       </c>
@@ -1433,7 +1442,7 @@
         <v>1997.7152581299345</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>9</v>
       </c>
@@ -1444,7 +1453,7 @@
         <v>240.67696765163419</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>10</v>
       </c>
@@ -1469,14 +1478,14 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
@@ -1499,7 +1508,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>7</v>
       </c>
@@ -1522,7 +1531,7 @@
         <v>3.0885108776335436E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>8</v>
       </c>
@@ -1545,7 +1554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>9</v>
       </c>
@@ -1568,7 +1577,7 @@
         <v>3.0835108270552154E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>10</v>
       </c>
@@ -1605,20 +1614,20 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C3" s="14"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B4" s="9" t="s">
         <v>1</v>
       </c>
@@ -1635,7 +1644,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B5" s="9">
         <v>1355555555</v>
       </c>
@@ -1673,7 +1682,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B6" s="9">
         <v>1455555555</v>
       </c>
@@ -1706,7 +1715,7 @@
       </c>
       <c r="J6" s="13"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B7" s="9">
         <v>1535555555</v>
       </c>
@@ -1739,7 +1748,7 @@
       </c>
       <c r="J7" s="13"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B8" s="9">
         <v>1545555555</v>
       </c>
@@ -1772,7 +1781,7 @@
       </c>
       <c r="J8" s="13"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9" s="9">
         <v>1553555555</v>
       </c>
@@ -1805,7 +1814,7 @@
       </c>
       <c r="J9" s="13"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10" s="9">
         <v>1554555555</v>
       </c>
@@ -1838,7 +1847,7 @@
       </c>
       <c r="J10" s="13"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11" s="9">
         <v>1555355555</v>
       </c>
@@ -1871,7 +1880,7 @@
       </c>
       <c r="J11" s="13"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B12" s="9">
         <v>1555455555</v>
       </c>
@@ -1904,7 +1913,7 @@
       </c>
       <c r="J12" s="13"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B13" s="9">
         <v>1555535555</v>
       </c>
@@ -1937,7 +1946,7 @@
       </c>
       <c r="J13" s="13"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B14" s="9">
         <v>1555545555</v>
       </c>
@@ -1970,7 +1979,7 @@
       </c>
       <c r="J14" s="13"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B15" s="9">
         <v>1555553555</v>
       </c>
@@ -2003,7 +2012,7 @@
       </c>
       <c r="J15" s="13"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B16" s="9">
         <v>1555554555</v>
       </c>
@@ -2036,7 +2045,7 @@
       </c>
       <c r="J16" s="13"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" s="9">
         <v>1555555355</v>
       </c>
@@ -2069,7 +2078,7 @@
       </c>
       <c r="J17" s="13"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" s="9">
         <v>1555555455</v>
       </c>
@@ -2102,7 +2111,7 @@
       </c>
       <c r="J18" s="13"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" s="9">
         <v>1555555535</v>
       </c>
@@ -2135,7 +2144,7 @@
       </c>
       <c r="J19" s="13"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" s="9">
         <v>1555555545</v>
       </c>
@@ -2168,7 +2177,7 @@
       </c>
       <c r="J20" s="13"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B21" s="9">
         <v>1555555553</v>
       </c>
@@ -2201,7 +2210,7 @@
       </c>
       <c r="J21" s="13"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" s="9">
         <v>1555555554</v>
       </c>
@@ -2234,7 +2243,7 @@
       </c>
       <c r="J22" s="13"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B23" s="9">
         <v>1555555555</v>
       </c>
@@ -2267,7 +2276,7 @@
       </c>
       <c r="J23" s="13"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B24" s="9">
         <v>1555555556</v>
       </c>
@@ -2299,7 +2308,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B25" s="9">
         <v>1555555557</v>
       </c>
@@ -2331,7 +2340,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B26" s="9">
         <v>1555555565</v>
       </c>
@@ -2363,7 +2372,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B27" s="9">
         <v>1555555575</v>
       </c>
@@ -2395,7 +2404,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B28" s="9">
         <v>1555555655</v>
       </c>
@@ -2427,7 +2436,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B29" s="9">
         <v>1555555755</v>
       </c>
@@ -2459,7 +2468,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B30" s="9">
         <v>1555556555</v>
       </c>
@@ -2491,7 +2500,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B31" s="9">
         <v>1555557555</v>
       </c>
@@ -2523,7 +2532,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B32" s="9">
         <v>1555565555</v>
       </c>
@@ -2555,7 +2564,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B33" s="9">
         <v>1555575555</v>
       </c>
@@ -2587,7 +2596,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B34" s="9">
         <v>1555655555</v>
       </c>
@@ -2619,7 +2628,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B35" s="9">
         <v>1555755555</v>
       </c>
@@ -2651,7 +2660,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B36" s="9">
         <v>1556555555</v>
       </c>
@@ -2683,7 +2692,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B37" s="9">
         <v>1557555555</v>
       </c>
@@ -2715,7 +2724,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B38" s="9">
         <v>1565555555</v>
       </c>
@@ -2747,7 +2756,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B39" s="9">
         <v>1575555555</v>
       </c>
@@ -2779,7 +2788,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B40" s="9">
         <v>1655555555</v>
       </c>
@@ -2811,7 +2820,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B41" s="9">
         <v>1755555555</v>
       </c>
@@ -2843,7 +2852,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B42" s="9">
         <v>2355555555</v>
       </c>
@@ -2875,7 +2884,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B43" s="9">
         <v>2455555555</v>
       </c>
@@ -2907,7 +2916,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B44" s="9">
         <v>2535555555</v>
       </c>
@@ -2939,7 +2948,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B45" s="9">
         <v>2545555555</v>
       </c>
@@ -2971,7 +2980,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B46" s="9">
         <v>2553555555</v>
       </c>
@@ -3003,7 +3012,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B47" s="9">
         <v>2554555555</v>
       </c>
@@ -3035,7 +3044,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B48" s="9">
         <v>2555355555</v>
       </c>
@@ -3067,7 +3076,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B49" s="9">
         <v>2555455555</v>
       </c>
@@ -3099,7 +3108,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B50" s="9">
         <v>2555535555</v>
       </c>
@@ -3131,7 +3140,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B51" s="9">
         <v>2555545555</v>
       </c>
@@ -3163,7 +3172,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B52" s="9">
         <v>2555553555</v>
       </c>
@@ -3195,7 +3204,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B53" s="9">
         <v>2555554555</v>
       </c>
@@ -3227,7 +3236,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B54" s="9">
         <v>2555555355</v>
       </c>
@@ -3259,7 +3268,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B55" s="9">
         <v>2555555455</v>
       </c>
@@ -3291,7 +3300,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B56" s="9">
         <v>2555555535</v>
       </c>
@@ -3323,7 +3332,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B57" s="9">
         <v>2555555545</v>
       </c>
@@ -3355,7 +3364,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B58" s="9">
         <v>2555555553</v>
       </c>
@@ -3387,7 +3396,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B59" s="9">
         <v>2555555554</v>
       </c>
@@ -3419,7 +3428,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B60" s="9">
         <v>2555555555</v>
       </c>
@@ -3451,7 +3460,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B61" s="9">
         <v>2555555556</v>
       </c>
@@ -3483,7 +3492,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B62" s="9">
         <v>2555555557</v>
       </c>
@@ -3515,7 +3524,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B63" s="9">
         <v>2555555565</v>
       </c>
@@ -3547,7 +3556,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B64" s="9">
         <v>2555555575</v>
       </c>
@@ -3579,7 +3588,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B65" s="9">
         <v>2555555655</v>
       </c>
@@ -3611,7 +3620,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B66" s="9">
         <v>2555555755</v>
       </c>
@@ -3643,7 +3652,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B67" s="9">
         <v>2555556555</v>
       </c>
@@ -3675,7 +3684,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B68" s="9">
         <v>2555557555</v>
       </c>
@@ -3707,7 +3716,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B69" s="9">
         <v>2555565555</v>
       </c>
@@ -3739,7 +3748,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B70" s="9">
         <v>2555575555</v>
       </c>
@@ -3771,7 +3780,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B71" s="9">
         <v>2555655555</v>
       </c>
@@ -3803,7 +3812,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B72" s="9">
         <v>2555755555</v>
       </c>
@@ -3835,7 +3844,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B73" s="9">
         <v>2556555555</v>
       </c>
@@ -3867,7 +3876,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B74" s="9">
         <v>2557555555</v>
       </c>
@@ -3899,7 +3908,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B75" s="9">
         <v>2565555555</v>
       </c>
@@ -3931,7 +3940,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B76" s="9">
         <v>2575555555</v>
       </c>
@@ -3963,7 +3972,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B77" s="9">
         <v>2655555555</v>
       </c>
@@ -3995,7 +4004,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B78" s="9">
         <v>2755555555</v>
       </c>
@@ -4027,7 +4036,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B79" s="9">
         <v>3355555555</v>
       </c>
@@ -4059,7 +4068,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B80" s="9">
         <v>3455555555</v>
       </c>
@@ -4091,7 +4100,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B81" s="9">
         <v>3535555555</v>
       </c>
@@ -4123,7 +4132,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B82" s="9">
         <v>3545555555</v>
       </c>
@@ -4155,7 +4164,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B83" s="9">
         <v>3553555555</v>
       </c>
@@ -4187,7 +4196,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B84" s="9">
         <v>3554555555</v>
       </c>
@@ -4219,7 +4228,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B85" s="9">
         <v>3555355555</v>
       </c>
@@ -4251,7 +4260,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B86" s="9">
         <v>3555455555</v>
       </c>
@@ -4283,7 +4292,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B87" s="9">
         <v>3555535555</v>
       </c>
@@ -4315,7 +4324,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B88" s="9">
         <v>3555545555</v>
       </c>
@@ -4347,7 +4356,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B89" s="9">
         <v>3555553555</v>
       </c>
@@ -4379,7 +4388,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B90" s="9">
         <v>3555554555</v>
       </c>
@@ -4411,7 +4420,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B91" s="9">
         <v>3555555355</v>
       </c>
@@ -4443,7 +4452,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B92" s="9">
         <v>3555555455</v>
       </c>
@@ -4475,7 +4484,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B93" s="9">
         <v>3555555535</v>
       </c>
@@ -4507,7 +4516,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B94" s="9">
         <v>3555555545</v>
       </c>
@@ -4539,7 +4548,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B95" s="9">
         <v>3555555553</v>
       </c>
@@ -4571,7 +4580,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B96" s="9">
         <v>3555555554</v>
       </c>
@@ -4603,7 +4612,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B97" s="9">
         <v>3555555555</v>
       </c>
@@ -4635,7 +4644,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B98" s="9">
         <v>3555555556</v>
       </c>
@@ -4667,7 +4676,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B99" s="9">
         <v>3555555557</v>
       </c>
@@ -4699,7 +4708,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B100" s="9">
         <v>3555555565</v>
       </c>
@@ -4731,7 +4740,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B101" s="9">
         <v>3555555575</v>
       </c>
@@ -4763,7 +4772,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B102" s="9">
         <v>3555555655</v>
       </c>
@@ -4795,7 +4804,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B103" s="9">
         <v>3555555755</v>
       </c>
@@ -4827,7 +4836,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="104" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B104" s="9">
         <v>3555556555</v>
       </c>
@@ -4859,7 +4868,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B105" s="9">
         <v>3555557555</v>
       </c>
@@ -4891,7 +4900,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B106" s="9">
         <v>3555565555</v>
       </c>
@@ -4923,7 +4932,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="107" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B107" s="9">
         <v>3555575555</v>
       </c>
@@ -4955,7 +4964,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B108" s="9">
         <v>3555655555</v>
       </c>
@@ -4987,7 +4996,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B109" s="9">
         <v>3555755555</v>
       </c>
@@ -5019,7 +5028,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B110" s="9">
         <v>3556555555</v>
       </c>
@@ -5051,7 +5060,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="111" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B111" s="9">
         <v>3557555555</v>
       </c>
@@ -5083,7 +5092,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="112" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B112" s="9">
         <v>3565555555</v>
       </c>
@@ -5115,7 +5124,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="113" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B113" s="9">
         <v>3575555555</v>
       </c>
@@ -5147,7 +5156,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="114" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B114" s="9">
         <v>3655555555</v>
       </c>
@@ -5179,7 +5188,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="115" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B115" s="9">
         <v>3755555555</v>
       </c>
@@ -5211,7 +5220,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="116" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B116" s="9">
         <v>4355555555</v>
       </c>
@@ -5243,7 +5252,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B117" s="9">
         <v>4455555555</v>
       </c>
@@ -5275,7 +5284,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B118" s="9">
         <v>4535555555</v>
       </c>
@@ -5307,7 +5316,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="119" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B119" s="9">
         <v>4545555555</v>
       </c>
@@ -5339,7 +5348,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B120" s="9">
         <v>4553555555</v>
       </c>
@@ -5371,7 +5380,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B121" s="9">
         <v>4554555555</v>
       </c>
@@ -5403,7 +5412,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="122" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B122" s="9">
         <v>4555355555</v>
       </c>
@@ -5435,7 +5444,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B123" s="9">
         <v>4555455555</v>
       </c>
@@ -5467,7 +5476,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="124" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B124" s="9">
         <v>4555535555</v>
       </c>
@@ -5499,7 +5508,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B125" s="9">
         <v>4555545555</v>
       </c>
@@ -5531,7 +5540,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="126" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B126" s="9">
         <v>4555553555</v>
       </c>
@@ -5563,7 +5572,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="127" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B127" s="9">
         <v>4555554555</v>
       </c>
@@ -5595,7 +5604,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="128" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B128" s="9">
         <v>4555555355</v>
       </c>
@@ -5627,7 +5636,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="129" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B129" s="9">
         <v>4555555455</v>
       </c>
@@ -5659,7 +5668,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="130" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B130" s="9">
         <v>4555555535</v>
       </c>
@@ -5691,7 +5700,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="131" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B131" s="9">
         <v>4555555545</v>
       </c>
@@ -5723,7 +5732,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="132" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B132" s="9">
         <v>4555555553</v>
       </c>
@@ -5755,7 +5764,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="133" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B133" s="9">
         <v>4555555554</v>
       </c>
@@ -5787,7 +5796,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B134" s="9">
         <v>4555555555</v>
       </c>
@@ -5819,7 +5828,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="135" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B135" s="9">
         <v>4555555556</v>
       </c>
@@ -5851,7 +5860,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="136" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B136" s="9">
         <v>4555555557</v>
       </c>
@@ -5883,7 +5892,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="137" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B137" s="9">
         <v>4555555565</v>
       </c>
@@ -5915,7 +5924,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="138" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B138" s="9">
         <v>4555555575</v>
       </c>
@@ -5947,7 +5956,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="139" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B139" s="9">
         <v>4555555655</v>
       </c>
@@ -5979,7 +5988,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="140" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B140" s="9">
         <v>4555555755</v>
       </c>
@@ -6011,7 +6020,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="141" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B141" s="9">
         <v>4555556555</v>
       </c>
@@ -6043,7 +6052,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="142" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B142" s="9">
         <v>4555557555</v>
       </c>
@@ -6075,7 +6084,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="143" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B143" s="9">
         <v>4555565555</v>
       </c>
@@ -6107,7 +6116,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="144" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B144" s="9">
         <v>4555575555</v>
       </c>
@@ -6139,7 +6148,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="145" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B145" s="9">
         <v>4555655555</v>
       </c>
@@ -6171,7 +6180,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="146" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B146" s="9">
         <v>4555755555</v>
       </c>
@@ -6203,7 +6212,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="147" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B147" s="9">
         <v>4556555555</v>
       </c>
@@ -6235,7 +6244,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="148" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B148" s="9">
         <v>4557555555</v>
       </c>
@@ -6267,7 +6276,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="149" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B149" s="9">
         <v>4565555555</v>
       </c>
@@ -6299,7 +6308,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="150" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B150" s="9">
         <v>4575555555</v>
       </c>
@@ -6331,7 +6340,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="151" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B151" s="9">
         <v>4655555555</v>
       </c>
@@ -6363,7 +6372,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="152" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B152" s="9">
         <v>4755555555</v>
       </c>
@@ -6409,13 +6418,13 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>32</v>
       </c>
@@ -6429,7 +6438,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="10">
         <v>1</v>
       </c>
@@ -6443,7 +6452,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="10">
         <v>2</v>
       </c>
@@ -6457,7 +6466,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="10">
         <v>3</v>
       </c>
@@ -6471,7 +6480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" s="10">
         <v>4</v>
       </c>
@@ -6485,7 +6494,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="F7" s="11">
         <v>7</v>
       </c>
@@ -6493,7 +6502,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>32</v>
       </c>
@@ -6501,7 +6510,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="2:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B13" s="13">
         <v>0</v>
       </c>
@@ -6509,7 +6518,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>1</v>
       </c>
@@ -6517,7 +6526,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15" s="13">
         <v>2</v>
       </c>
@@ -6525,7 +6534,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B16" s="13">
         <v>3</v>
       </c>
@@ -6533,7 +6542,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" s="13">
         <v>4</v>
       </c>
@@ -6541,7 +6550,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" s="13">
         <v>5</v>
       </c>
@@ -6549,7 +6558,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" s="13">
         <v>6</v>
       </c>
@@ -6557,7 +6566,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" s="13">
         <v>7</v>
       </c>
@@ -6565,7 +6574,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" s="13">
         <v>8</v>
       </c>
@@ -6573,7 +6582,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" s="13">
         <v>9</v>
       </c>
@@ -6596,17 +6605,17 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:V149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
@@ -6630,7 +6639,7 @@
         <v>2</v>
       </c>
       <c r="L1" s="17" t="s">
-        <v>3</v>
+        <v>69</v>
       </c>
       <c r="M1" s="17" t="s">
         <v>4</v>
@@ -6639,16 +6648,16 @@
         <v>5</v>
       </c>
       <c r="O1" s="17" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="P1" s="17" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="Q1" s="17" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="R1" s="17" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="S1" s="17" t="s">
         <v>45</v>
@@ -6658,7 +6667,7 @@
       </c>
       <c r="V1" s="17"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="13">
         <v>1355555555</v>
       </c>
@@ -6722,7 +6731,7 @@
       </c>
       <c r="V2" s="17"/>
     </row>
-    <row r="3" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>1455555555</v>
       </c>
@@ -6786,7 +6795,7 @@
       </c>
       <c r="V3" s="17"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>1535555555</v>
       </c>
@@ -6850,7 +6859,7 @@
       </c>
       <c r="V4" s="17"/>
     </row>
-    <row r="5" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>1545555555</v>
       </c>
@@ -6914,7 +6923,7 @@
       </c>
       <c r="V5" s="17"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>1553555555</v>
       </c>
@@ -6978,7 +6987,7 @@
       </c>
       <c r="V6" s="17"/>
     </row>
-    <row r="7" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>1554555555</v>
       </c>
@@ -7042,7 +7051,7 @@
       </c>
       <c r="V7" s="17"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>1555355555</v>
       </c>
@@ -7106,7 +7115,7 @@
       </c>
       <c r="V8" s="17"/>
     </row>
-    <row r="9" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>1555455555</v>
       </c>
@@ -7170,7 +7179,7 @@
       </c>
       <c r="V9" s="17"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>1555535555</v>
       </c>
@@ -7234,7 +7243,7 @@
       </c>
       <c r="V10" s="17"/>
     </row>
-    <row r="11" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <v>1555545555</v>
       </c>
@@ -7298,7 +7307,7 @@
       </c>
       <c r="V11" s="17"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <v>1555553555</v>
       </c>
@@ -7362,7 +7371,7 @@
       </c>
       <c r="V12" s="17"/>
     </row>
-    <row r="13" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13">
         <v>1555554555</v>
       </c>
@@ -7426,7 +7435,7 @@
       </c>
       <c r="V13" s="17"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="13">
         <v>1555555355</v>
       </c>
@@ -7490,7 +7499,7 @@
       </c>
       <c r="V14" s="17"/>
     </row>
-    <row r="15" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="13">
         <v>1555555455</v>
       </c>
@@ -7554,7 +7563,7 @@
       </c>
       <c r="V15" s="17"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="13">
         <v>1555555535</v>
       </c>
@@ -7618,7 +7627,7 @@
       </c>
       <c r="V16" s="17"/>
     </row>
-    <row r="17" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13">
         <v>1555555545</v>
       </c>
@@ -7682,7 +7691,7 @@
       </c>
       <c r="V17" s="17"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="13">
         <v>1555555553</v>
       </c>
@@ -7746,7 +7755,7 @@
       </c>
       <c r="V18" s="17"/>
     </row>
-    <row r="19" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13">
         <v>1555555554</v>
       </c>
@@ -7810,7 +7819,7 @@
       </c>
       <c r="V19" s="17"/>
     </row>
-    <row r="20" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13">
         <v>1555555555</v>
       </c>
@@ -7874,7 +7883,7 @@
       </c>
       <c r="V20" s="17"/>
     </row>
-    <row r="21" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13">
         <v>1555555556</v>
       </c>
@@ -7938,7 +7947,7 @@
       </c>
       <c r="V21" s="17"/>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" s="13">
         <v>1555555557</v>
       </c>
@@ -8002,7 +8011,7 @@
       </c>
       <c r="V22" s="17"/>
     </row>
-    <row r="23" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13">
         <v>1555555565</v>
       </c>
@@ -8066,7 +8075,7 @@
       </c>
       <c r="V23" s="17"/>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" s="13">
         <v>1555555575</v>
       </c>
@@ -8130,7 +8139,7 @@
       </c>
       <c r="V24" s="17"/>
     </row>
-    <row r="25" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13">
         <v>1555555655</v>
       </c>
@@ -8194,7 +8203,7 @@
       </c>
       <c r="V25" s="17"/>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" s="13">
         <v>1555555755</v>
       </c>
@@ -8258,7 +8267,7 @@
       </c>
       <c r="V26" s="17"/>
     </row>
-    <row r="27" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13">
         <v>1555556555</v>
       </c>
@@ -8322,7 +8331,7 @@
       </c>
       <c r="V27" s="17"/>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="13">
         <v>1555557555</v>
       </c>
@@ -8386,7 +8395,7 @@
       </c>
       <c r="V28" s="17"/>
     </row>
-    <row r="29" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="13">
         <v>1555565555</v>
       </c>
@@ -8450,7 +8459,7 @@
       </c>
       <c r="V29" s="17"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" s="13">
         <v>1555575555</v>
       </c>
@@ -8514,7 +8523,7 @@
       </c>
       <c r="V30" s="17"/>
     </row>
-    <row r="31" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="13">
         <v>1555655555</v>
       </c>
@@ -8578,7 +8587,7 @@
       </c>
       <c r="V31" s="17"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" s="13">
         <v>1555755555</v>
       </c>
@@ -8642,7 +8651,7 @@
       </c>
       <c r="V32" s="17"/>
     </row>
-    <row r="33" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="13">
         <v>1556555555</v>
       </c>
@@ -8706,7 +8715,7 @@
       </c>
       <c r="V33" s="17"/>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A34" s="13">
         <v>1557555555</v>
       </c>
@@ -8770,7 +8779,7 @@
       </c>
       <c r="V34" s="17"/>
     </row>
-    <row r="35" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="13">
         <v>1565555555</v>
       </c>
@@ -8834,7 +8843,7 @@
       </c>
       <c r="V35" s="17"/>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A36" s="13">
         <v>1575555555</v>
       </c>
@@ -8898,7 +8907,7 @@
       </c>
       <c r="V36" s="17"/>
     </row>
-    <row r="37" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="13">
         <v>1655555555</v>
       </c>
@@ -8962,7 +8971,7 @@
       </c>
       <c r="V37" s="17"/>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A38" s="13">
         <v>1755555555</v>
       </c>
@@ -9026,7 +9035,7 @@
       </c>
       <c r="V38" s="17"/>
     </row>
-    <row r="39" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="13">
         <v>2355555555</v>
       </c>
@@ -9090,7 +9099,7 @@
       </c>
       <c r="V39" s="17"/>
     </row>
-    <row r="40" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="13">
         <v>2455555555</v>
       </c>
@@ -9154,7 +9163,7 @@
       </c>
       <c r="V40" s="17"/>
     </row>
-    <row r="41" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="13">
         <v>2535555555</v>
       </c>
@@ -9218,7 +9227,7 @@
       </c>
       <c r="V41" s="17"/>
     </row>
-    <row r="42" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="13">
         <v>2545555555</v>
       </c>
@@ -9282,7 +9291,7 @@
       </c>
       <c r="V42" s="17"/>
     </row>
-    <row r="43" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="13">
         <v>2553555555</v>
       </c>
@@ -9346,7 +9355,7 @@
       </c>
       <c r="V43" s="17"/>
     </row>
-    <row r="44" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="13">
         <v>2554555555</v>
       </c>
@@ -9410,7 +9419,7 @@
       </c>
       <c r="V44" s="17"/>
     </row>
-    <row r="45" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="13">
         <v>2555355555</v>
       </c>
@@ -9474,7 +9483,7 @@
       </c>
       <c r="V45" s="17"/>
     </row>
-    <row r="46" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="13">
         <v>2555455555</v>
       </c>
@@ -9538,7 +9547,7 @@
       </c>
       <c r="V46" s="17"/>
     </row>
-    <row r="47" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="13">
         <v>2555535555</v>
       </c>
@@ -9602,7 +9611,7 @@
       </c>
       <c r="V47" s="17"/>
     </row>
-    <row r="48" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="13">
         <v>2555545555</v>
       </c>
@@ -9666,7 +9675,7 @@
       </c>
       <c r="V48" s="17"/>
     </row>
-    <row r="49" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="13">
         <v>2555553555</v>
       </c>
@@ -9730,7 +9739,7 @@
       </c>
       <c r="V49" s="17"/>
     </row>
-    <row r="50" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="13">
         <v>2555554555</v>
       </c>
@@ -9794,7 +9803,7 @@
       </c>
       <c r="V50" s="17"/>
     </row>
-    <row r="51" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="13">
         <v>2555555355</v>
       </c>
@@ -9858,7 +9867,7 @@
       </c>
       <c r="V51" s="17"/>
     </row>
-    <row r="52" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="13">
         <v>2555555455</v>
       </c>
@@ -9922,7 +9931,7 @@
       </c>
       <c r="V52" s="17"/>
     </row>
-    <row r="53" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="13">
         <v>2555555535</v>
       </c>
@@ -9986,7 +9995,7 @@
       </c>
       <c r="V53" s="17"/>
     </row>
-    <row r="54" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="13">
         <v>2555555545</v>
       </c>
@@ -10050,7 +10059,7 @@
       </c>
       <c r="V54" s="17"/>
     </row>
-    <row r="55" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="13">
         <v>2555555553</v>
       </c>
@@ -10114,7 +10123,7 @@
       </c>
       <c r="V55" s="17"/>
     </row>
-    <row r="56" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="13">
         <v>2555555554</v>
       </c>
@@ -10178,7 +10187,7 @@
       </c>
       <c r="V56" s="17"/>
     </row>
-    <row r="57" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="13">
         <v>2555555555</v>
       </c>
@@ -10242,7 +10251,7 @@
       </c>
       <c r="V57" s="17"/>
     </row>
-    <row r="58" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="13">
         <v>2555555556</v>
       </c>
@@ -10306,7 +10315,7 @@
       </c>
       <c r="V58" s="17"/>
     </row>
-    <row r="59" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="13">
         <v>2555555557</v>
       </c>
@@ -10370,7 +10379,7 @@
       </c>
       <c r="V59" s="17"/>
     </row>
-    <row r="60" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="13">
         <v>2555555565</v>
       </c>
@@ -10434,7 +10443,7 @@
       </c>
       <c r="V60" s="17"/>
     </row>
-    <row r="61" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="13">
         <v>2555555575</v>
       </c>
@@ -10498,7 +10507,7 @@
       </c>
       <c r="V61" s="17"/>
     </row>
-    <row r="62" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="13">
         <v>2555555655</v>
       </c>
@@ -10562,7 +10571,7 @@
       </c>
       <c r="V62" s="17"/>
     </row>
-    <row r="63" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="13">
         <v>2555555755</v>
       </c>
@@ -10626,7 +10635,7 @@
       </c>
       <c r="V63" s="17"/>
     </row>
-    <row r="64" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="13">
         <v>2555556555</v>
       </c>
@@ -10690,7 +10699,7 @@
       </c>
       <c r="V64" s="17"/>
     </row>
-    <row r="65" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="13">
         <v>2555557555</v>
       </c>
@@ -10754,7 +10763,7 @@
       </c>
       <c r="V65" s="17"/>
     </row>
-    <row r="66" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="13">
         <v>2555565555</v>
       </c>
@@ -10818,7 +10827,7 @@
       </c>
       <c r="V66" s="17"/>
     </row>
-    <row r="67" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="13">
         <v>2555575555</v>
       </c>
@@ -10882,7 +10891,7 @@
       </c>
       <c r="V67" s="17"/>
     </row>
-    <row r="68" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="13">
         <v>2555655555</v>
       </c>
@@ -10946,7 +10955,7 @@
       </c>
       <c r="V68" s="17"/>
     </row>
-    <row r="69" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="13">
         <v>2555755555</v>
       </c>
@@ -11010,7 +11019,7 @@
       </c>
       <c r="V69" s="17"/>
     </row>
-    <row r="70" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="13">
         <v>2556555555</v>
       </c>
@@ -11074,7 +11083,7 @@
       </c>
       <c r="V70" s="17"/>
     </row>
-    <row r="71" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="13">
         <v>2557555555</v>
       </c>
@@ -11138,7 +11147,7 @@
       </c>
       <c r="V71" s="17"/>
     </row>
-    <row r="72" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="13">
         <v>2565555555</v>
       </c>
@@ -11202,7 +11211,7 @@
       </c>
       <c r="V72" s="17"/>
     </row>
-    <row r="73" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="13">
         <v>2575555555</v>
       </c>
@@ -11266,7 +11275,7 @@
       </c>
       <c r="V73" s="17"/>
     </row>
-    <row r="74" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="13">
         <v>2655555555</v>
       </c>
@@ -11330,7 +11339,7 @@
       </c>
       <c r="V74" s="17"/>
     </row>
-    <row r="75" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="13">
         <v>2755555555</v>
       </c>
@@ -11394,7 +11403,7 @@
       </c>
       <c r="V75" s="17"/>
     </row>
-    <row r="76" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="13">
         <v>3355555555</v>
       </c>
@@ -11458,7 +11467,7 @@
       </c>
       <c r="V76" s="17"/>
     </row>
-    <row r="77" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="13">
         <v>3455555555</v>
       </c>
@@ -11522,7 +11531,7 @@
       </c>
       <c r="V77" s="17"/>
     </row>
-    <row r="78" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="13">
         <v>3535555555</v>
       </c>
@@ -11586,7 +11595,7 @@
       </c>
       <c r="V78" s="17"/>
     </row>
-    <row r="79" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="13">
         <v>3545555555</v>
       </c>
@@ -11650,7 +11659,7 @@
       </c>
       <c r="V79" s="17"/>
     </row>
-    <row r="80" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="13">
         <v>3553555555</v>
       </c>
@@ -11714,7 +11723,7 @@
       </c>
       <c r="V80" s="17"/>
     </row>
-    <row r="81" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="13">
         <v>3554555555</v>
       </c>
@@ -11778,7 +11787,7 @@
       </c>
       <c r="V81" s="17"/>
     </row>
-    <row r="82" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="13">
         <v>3555355555</v>
       </c>
@@ -11842,7 +11851,7 @@
       </c>
       <c r="V82" s="17"/>
     </row>
-    <row r="83" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="13">
         <v>3555455555</v>
       </c>
@@ -11906,7 +11915,7 @@
       </c>
       <c r="V83" s="17"/>
     </row>
-    <row r="84" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="13">
         <v>3555535555</v>
       </c>
@@ -11970,7 +11979,7 @@
       </c>
       <c r="V84" s="17"/>
     </row>
-    <row r="85" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="13">
         <v>3555545555</v>
       </c>
@@ -12034,7 +12043,7 @@
       </c>
       <c r="V85" s="17"/>
     </row>
-    <row r="86" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="13">
         <v>3555553555</v>
       </c>
@@ -12098,7 +12107,7 @@
       </c>
       <c r="V86" s="17"/>
     </row>
-    <row r="87" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="13">
         <v>3555554555</v>
       </c>
@@ -12162,7 +12171,7 @@
       </c>
       <c r="V87" s="17"/>
     </row>
-    <row r="88" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="13">
         <v>3555555355</v>
       </c>
@@ -12226,7 +12235,7 @@
       </c>
       <c r="V88" s="17"/>
     </row>
-    <row r="89" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="13">
         <v>3555555455</v>
       </c>
@@ -12290,7 +12299,7 @@
       </c>
       <c r="V89" s="17"/>
     </row>
-    <row r="90" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" s="13">
         <v>3555555535</v>
       </c>
@@ -12354,7 +12363,7 @@
       </c>
       <c r="V90" s="17"/>
     </row>
-    <row r="91" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" s="13">
         <v>3555555545</v>
       </c>
@@ -12418,7 +12427,7 @@
       </c>
       <c r="V91" s="17"/>
     </row>
-    <row r="92" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="13">
         <v>3555555553</v>
       </c>
@@ -12482,7 +12491,7 @@
       </c>
       <c r="V92" s="17"/>
     </row>
-    <row r="93" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" s="13">
         <v>3555555554</v>
       </c>
@@ -12546,7 +12555,7 @@
       </c>
       <c r="V93" s="17"/>
     </row>
-    <row r="94" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" s="13">
         <v>3555555555</v>
       </c>
@@ -12610,7 +12619,7 @@
       </c>
       <c r="V94" s="17"/>
     </row>
-    <row r="95" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" s="13">
         <v>3555555556</v>
       </c>
@@ -12674,7 +12683,7 @@
       </c>
       <c r="V95" s="17"/>
     </row>
-    <row r="96" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" s="13">
         <v>3555555557</v>
       </c>
@@ -12738,7 +12747,7 @@
       </c>
       <c r="V96" s="17"/>
     </row>
-    <row r="97" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" s="13">
         <v>3555555565</v>
       </c>
@@ -12802,7 +12811,7 @@
       </c>
       <c r="V97" s="17"/>
     </row>
-    <row r="98" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="13">
         <v>3555555575</v>
       </c>
@@ -12866,7 +12875,7 @@
       </c>
       <c r="V98" s="17"/>
     </row>
-    <row r="99" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" s="13">
         <v>3555555655</v>
       </c>
@@ -12930,7 +12939,7 @@
       </c>
       <c r="V99" s="17"/>
     </row>
-    <row r="100" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" s="13">
         <v>3555555755</v>
       </c>
@@ -12994,7 +13003,7 @@
       </c>
       <c r="V100" s="17"/>
     </row>
-    <row r="101" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" s="13">
         <v>3555556555</v>
       </c>
@@ -13058,7 +13067,7 @@
       </c>
       <c r="V101" s="17"/>
     </row>
-    <row r="102" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" s="13">
         <v>3555557555</v>
       </c>
@@ -13122,7 +13131,7 @@
       </c>
       <c r="V102" s="17"/>
     </row>
-    <row r="103" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" s="13">
         <v>3555565555</v>
       </c>
@@ -13186,7 +13195,7 @@
       </c>
       <c r="V103" s="17"/>
     </row>
-    <row r="104" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="13">
         <v>3555575555</v>
       </c>
@@ -13250,7 +13259,7 @@
       </c>
       <c r="V104" s="17"/>
     </row>
-    <row r="105" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" s="13">
         <v>3555655555</v>
       </c>
@@ -13314,7 +13323,7 @@
       </c>
       <c r="V105" s="17"/>
     </row>
-    <row r="106" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="13">
         <v>3555755555</v>
       </c>
@@ -13378,7 +13387,7 @@
       </c>
       <c r="V106" s="17"/>
     </row>
-    <row r="107" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" s="13">
         <v>3556555555</v>
       </c>
@@ -13442,7 +13451,7 @@
       </c>
       <c r="V107" s="17"/>
     </row>
-    <row r="108" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" s="13">
         <v>3557555555</v>
       </c>
@@ -13506,7 +13515,7 @@
       </c>
       <c r="V108" s="17"/>
     </row>
-    <row r="109" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" s="13">
         <v>3565555555</v>
       </c>
@@ -13570,7 +13579,7 @@
       </c>
       <c r="V109" s="17"/>
     </row>
-    <row r="110" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" s="13">
         <v>3575555555</v>
       </c>
@@ -13634,7 +13643,7 @@
       </c>
       <c r="V110" s="17"/>
     </row>
-    <row r="111" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" s="13">
         <v>3655555555</v>
       </c>
@@ -13698,7 +13707,7 @@
       </c>
       <c r="V111" s="17"/>
     </row>
-    <row r="112" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" s="13">
         <v>3755555555</v>
       </c>
@@ -13762,7 +13771,7 @@
       </c>
       <c r="V112" s="17"/>
     </row>
-    <row r="113" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" s="13">
         <v>4355555555</v>
       </c>
@@ -13826,7 +13835,7 @@
       </c>
       <c r="V113" s="17"/>
     </row>
-    <row r="114" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" s="13">
         <v>4455555555</v>
       </c>
@@ -13890,7 +13899,7 @@
       </c>
       <c r="V114" s="17"/>
     </row>
-    <row r="115" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" s="13">
         <v>4535555555</v>
       </c>
@@ -13954,7 +13963,7 @@
       </c>
       <c r="V115" s="17"/>
     </row>
-    <row r="116" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="13">
         <v>4545555555</v>
       </c>
@@ -14018,7 +14027,7 @@
       </c>
       <c r="V116" s="17"/>
     </row>
-    <row r="117" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="13">
         <v>4553555555</v>
       </c>
@@ -14082,7 +14091,7 @@
       </c>
       <c r="V117" s="17"/>
     </row>
-    <row r="118" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" s="13">
         <v>4554555555</v>
       </c>
@@ -14146,7 +14155,7 @@
       </c>
       <c r="V118" s="17"/>
     </row>
-    <row r="119" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" s="13">
         <v>4555355555</v>
       </c>
@@ -14210,7 +14219,7 @@
       </c>
       <c r="V119" s="17"/>
     </row>
-    <row r="120" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" s="13">
         <v>4555455555</v>
       </c>
@@ -14274,7 +14283,7 @@
       </c>
       <c r="V120" s="17"/>
     </row>
-    <row r="121" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="13">
         <v>4555535555</v>
       </c>
@@ -14338,7 +14347,7 @@
       </c>
       <c r="V121" s="17"/>
     </row>
-    <row r="122" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" s="13">
         <v>4555545555</v>
       </c>
@@ -14402,7 +14411,7 @@
       </c>
       <c r="V122" s="17"/>
     </row>
-    <row r="123" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" s="13">
         <v>4555553555</v>
       </c>
@@ -14466,7 +14475,7 @@
       </c>
       <c r="V123" s="17"/>
     </row>
-    <row r="124" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" s="13">
         <v>4555554555</v>
       </c>
@@ -14530,7 +14539,7 @@
       </c>
       <c r="V124" s="17"/>
     </row>
-    <row r="125" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" s="13">
         <v>4555555355</v>
       </c>
@@ -14594,7 +14603,7 @@
       </c>
       <c r="V125" s="17"/>
     </row>
-    <row r="126" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" s="13">
         <v>4555555455</v>
       </c>
@@ -14658,7 +14667,7 @@
       </c>
       <c r="V126" s="17"/>
     </row>
-    <row r="127" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" s="13">
         <v>4555555535</v>
       </c>
@@ -14722,7 +14731,7 @@
       </c>
       <c r="V127" s="17"/>
     </row>
-    <row r="128" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" s="13">
         <v>4555555545</v>
       </c>
@@ -14786,7 +14795,7 @@
       </c>
       <c r="V128" s="17"/>
     </row>
-    <row r="129" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" s="13">
         <v>4555555553</v>
       </c>
@@ -14850,7 +14859,7 @@
       </c>
       <c r="V129" s="17"/>
     </row>
-    <row r="130" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" s="13">
         <v>4555555554</v>
       </c>
@@ -14914,7 +14923,7 @@
       </c>
       <c r="V130" s="17"/>
     </row>
-    <row r="131" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" s="13">
         <v>4555555555</v>
       </c>
@@ -14978,7 +14987,7 @@
       </c>
       <c r="V131" s="17"/>
     </row>
-    <row r="132" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" s="13">
         <v>4555555556</v>
       </c>
@@ -15042,7 +15051,7 @@
       </c>
       <c r="V132" s="17"/>
     </row>
-    <row r="133" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" s="13">
         <v>4555555557</v>
       </c>
@@ -15106,7 +15115,7 @@
       </c>
       <c r="V133" s="17"/>
     </row>
-    <row r="134" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" s="13">
         <v>4555555565</v>
       </c>
@@ -15170,7 +15179,7 @@
       </c>
       <c r="V134" s="17"/>
     </row>
-    <row r="135" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" s="13">
         <v>4555555575</v>
       </c>
@@ -15234,7 +15243,7 @@
       </c>
       <c r="V135" s="17"/>
     </row>
-    <row r="136" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" s="13">
         <v>4555555655</v>
       </c>
@@ -15298,7 +15307,7 @@
       </c>
       <c r="V136" s="17"/>
     </row>
-    <row r="137" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" s="13">
         <v>4555555755</v>
       </c>
@@ -15362,7 +15371,7 @@
       </c>
       <c r="V137" s="17"/>
     </row>
-    <row r="138" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" s="13">
         <v>4555556555</v>
       </c>
@@ -15426,7 +15435,7 @@
       </c>
       <c r="V138" s="17"/>
     </row>
-    <row r="139" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" s="13">
         <v>4555557555</v>
       </c>
@@ -15490,7 +15499,7 @@
       </c>
       <c r="V139" s="17"/>
     </row>
-    <row r="140" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" s="13">
         <v>4555565555</v>
       </c>
@@ -15554,7 +15563,7 @@
       </c>
       <c r="V140" s="17"/>
     </row>
-    <row r="141" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" s="13">
         <v>4555575555</v>
       </c>
@@ -15618,7 +15627,7 @@
       </c>
       <c r="V141" s="17"/>
     </row>
-    <row r="142" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" s="13">
         <v>4555655555</v>
       </c>
@@ -15682,7 +15691,7 @@
       </c>
       <c r="V142" s="17"/>
     </row>
-    <row r="143" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" s="13">
         <v>4555755555</v>
       </c>
@@ -15746,7 +15755,7 @@
       </c>
       <c r="V143" s="17"/>
     </row>
-    <row r="144" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" s="13">
         <v>4556555555</v>
       </c>
@@ -15810,7 +15819,7 @@
       </c>
       <c r="V144" s="17"/>
     </row>
-    <row r="145" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" s="13">
         <v>4557555555</v>
       </c>
@@ -15874,7 +15883,7 @@
       </c>
       <c r="V145" s="17"/>
     </row>
-    <row r="146" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" s="13">
         <v>4565555555</v>
       </c>
@@ -15938,7 +15947,7 @@
       </c>
       <c r="V146" s="17"/>
     </row>
-    <row r="147" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" s="13">
         <v>4575555555</v>
       </c>
@@ -16002,7 +16011,7 @@
       </c>
       <c r="V147" s="17"/>
     </row>
-    <row r="148" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" s="13">
         <v>4655555555</v>
       </c>
@@ -16065,7 +16074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:22" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" s="13">
         <v>4755555555</v>
       </c>
@@ -16155,50 +16164,50 @@
       <selection activeCell="AO29" sqref="AO29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="11.42578125" style="17"/>
-    <col min="7" max="7" width="2.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" style="17"/>
+    <col min="7" max="7" width="2.33203125" customWidth="1"/>
     <col min="8" max="15" width="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="2" customWidth="1"/>
     <col min="17" max="24" width="2" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="2" customWidth="1"/>
     <col min="26" max="27" width="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="29" max="33" width="2" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="2" customWidth="1"/>
     <col min="35" max="36" width="2" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="39" max="41" width="2" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="2.140625" customWidth="1"/>
+    <col min="42" max="42" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="2.109375" customWidth="1"/>
     <col min="44" max="45" width="2" bestFit="1" customWidth="1"/>
-    <col min="46" max="49" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="49" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="50" max="51" width="2" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="2.140625" customWidth="1"/>
+    <col min="52" max="52" width="2.109375" customWidth="1"/>
     <col min="53" max="54" width="2" bestFit="1" customWidth="1"/>
-    <col min="55" max="58" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="55" max="58" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="59" max="60" width="2" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="2.28515625" customWidth="1"/>
+    <col min="61" max="61" width="2.33203125" customWidth="1"/>
     <col min="62" max="63" width="2" bestFit="1" customWidth="1"/>
-    <col min="64" max="67" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="64" max="67" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="68" max="69" width="2" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="2.5703125" customWidth="1"/>
+    <col min="70" max="70" width="2.5546875" customWidth="1"/>
     <col min="71" max="72" width="2" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="5" bestFit="1" customWidth="1"/>
-    <col min="75" max="78" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="75" max="78" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="79" max="79" width="2" customWidth="1"/>
     <col min="80" max="81" width="2" bestFit="1" customWidth="1"/>
-    <col min="82" max="87" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="2.42578125" customWidth="1"/>
+    <col min="82" max="87" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="2.44140625" customWidth="1"/>
     <col min="89" max="90" width="2" bestFit="1" customWidth="1"/>
-    <col min="91" max="94" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="91" max="94" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="95" max="95" width="2" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="5.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>1</v>
       </c>
@@ -16245,7 +16254,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A2" s="17">
         <v>1355555555</v>
       </c>
@@ -16625,7 +16634,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A3" s="17">
         <v>1535555555</v>
       </c>
@@ -17005,7 +17014,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A4" s="17">
         <v>1553555555</v>
       </c>
@@ -17385,7 +17394,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A5" s="17">
         <v>1555355555</v>
       </c>
@@ -17765,7 +17774,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A6" s="17">
         <v>1555535555</v>
       </c>
@@ -18145,7 +18154,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A7" s="17">
         <v>1555553555</v>
       </c>
@@ -18525,7 +18534,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A8" s="17">
         <v>1555555355</v>
       </c>
@@ -18905,7 +18914,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A9" s="17">
         <v>1555555535</v>
       </c>
@@ -19285,7 +19294,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A10" s="17">
         <v>1555555553</v>
       </c>
@@ -19665,7 +19674,7 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A11" s="17">
         <v>1555555557</v>
       </c>
@@ -20045,7 +20054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A12" s="17">
         <v>1555555575</v>
       </c>
@@ -20425,7 +20434,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A13" s="17">
         <v>1555555755</v>
       </c>
@@ -20805,7 +20814,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A14" s="17">
         <v>1555557555</v>
       </c>
@@ -21185,7 +21194,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A15" s="17">
         <v>1555575555</v>
       </c>
@@ -21565,7 +21574,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A16" s="17">
         <v>1555755555</v>
       </c>
@@ -21945,7 +21954,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A17" s="17">
         <v>1557555555</v>
       </c>
@@ -22325,7 +22334,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A18" s="17">
         <v>1575555555</v>
       </c>
@@ -22705,7 +22714,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A19" s="17">
         <v>1755555555</v>
       </c>
@@ -23098,9 +23107,9 @@
       <selection sqref="A1:T19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>1</v>
       </c>
@@ -23152,7 +23161,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="17">
         <v>1355555555</v>
       </c>
@@ -23210,7 +23219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="17">
         <v>1535555555</v>
       </c>
@@ -23268,7 +23277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="17">
         <v>1553555555</v>
       </c>
@@ -23326,7 +23335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="17">
         <v>1555355555</v>
       </c>
@@ -23384,7 +23393,7 @@
         <v>-0.22</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="17">
         <v>1555535555</v>
       </c>
@@ -23442,7 +23451,7 @@
         <v>-0.06</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="17">
         <v>1555553555</v>
       </c>
@@ -23500,7 +23509,7 @@
         <v>-0.11</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="17">
         <v>1555555355</v>
       </c>
@@ -23558,7 +23567,7 @@
         <v>-0.12</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="17">
         <v>1555555535</v>
       </c>
@@ -23616,7 +23625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="17">
         <v>1555555553</v>
       </c>
@@ -23674,7 +23683,7 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="17">
         <v>1555555557</v>
       </c>
@@ -23732,7 +23741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="17">
         <v>1555555575</v>
       </c>
@@ -23790,7 +23799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="17">
         <v>1555555755</v>
       </c>
@@ -23848,7 +23857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="17">
         <v>1555557555</v>
       </c>
@@ -23906,7 +23915,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="17">
         <v>1555575555</v>
       </c>
@@ -23964,7 +23973,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="17">
         <v>1555755555</v>
       </c>
@@ -24022,7 +24031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="17">
         <v>1557555555</v>
       </c>
@@ -24080,7 +24089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="17">
         <v>1575555555</v>
       </c>
@@ -24138,7 +24147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="17">
         <v>1755555555</v>
       </c>

</xml_diff>